<commit_message>
Add DEMOG variables to helper files
added NOM, NIM & Natural Increase variables
</commit_message>
<xml_diff>
--- a/data processing/Input Files/List_of_Indicators.xlsx
+++ b/data processing/Input Files/List_of_Indicators.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\BIS Consultancy\Product Development\Scenarios_Dashboard\Data Processing\Input Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcrook\Documents\scenario_dashboard\data processing\Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACEED45-3A38-40EA-9DF0-A5F5F40FD70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC660A9C-CBFE-4B5B-985C-CC1F7F94C794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="9060" windowWidth="23256" windowHeight="12576" xr2:uid="{794FE58A-84D8-4721-BA4E-C54580252300}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{794FE58A-84D8-4721-BA4E-C54580252300}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="328">
   <si>
     <t>POPTOTTACT</t>
   </si>
@@ -930,6 +930,96 @@
   </si>
   <si>
     <t>CPAD_0N</t>
+  </si>
+  <si>
+    <t>DEMOG</t>
+  </si>
+  <si>
+    <t>NSWNIMTOT</t>
+  </si>
+  <si>
+    <t>NIMTOT</t>
+  </si>
+  <si>
+    <t>NSWNOMTOT</t>
+  </si>
+  <si>
+    <t>NOMTOT</t>
+  </si>
+  <si>
+    <t>VICNIMTOT</t>
+  </si>
+  <si>
+    <t>VICNOMTOT</t>
+  </si>
+  <si>
+    <t>QLDNIMTOT</t>
+  </si>
+  <si>
+    <t>QLDNOMTOT</t>
+  </si>
+  <si>
+    <t>NSWNATTOT</t>
+  </si>
+  <si>
+    <t>NATTOT</t>
+  </si>
+  <si>
+    <t>VICNATTOT</t>
+  </si>
+  <si>
+    <t>QLDNATTOT</t>
+  </si>
+  <si>
+    <t>ACTNIMTOT</t>
+  </si>
+  <si>
+    <t>ACTNOMTOT</t>
+  </si>
+  <si>
+    <t>ACTNATTOT</t>
+  </si>
+  <si>
+    <t>TASNIMTOT</t>
+  </si>
+  <si>
+    <t>TASNOMTOT</t>
+  </si>
+  <si>
+    <t>TASNATTOT</t>
+  </si>
+  <si>
+    <t>SANIMTOT</t>
+  </si>
+  <si>
+    <t>SANOMTOT</t>
+  </si>
+  <si>
+    <t>SANATTOT</t>
+  </si>
+  <si>
+    <t>NTNIMTOT</t>
+  </si>
+  <si>
+    <t>NTNOMTOT</t>
+  </si>
+  <si>
+    <t>NTNATTOT</t>
+  </si>
+  <si>
+    <t>WANIMTOT</t>
+  </si>
+  <si>
+    <t>WANOMTOT</t>
+  </si>
+  <si>
+    <t>WANATTOT</t>
+  </si>
+  <si>
+    <t>AUSNOMTOT</t>
+  </si>
+  <si>
+    <t>AUSNATTOT</t>
   </si>
 </sst>
 </file>
@@ -1304,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5594264D-85FA-45F5-B682-9D38B256CF42}">
-  <dimension ref="A1:F259"/>
+  <dimension ref="A1:F285"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="F288" sqref="F288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6308,7 +6398,7 @@
         <v>271</v>
       </c>
       <c r="D238" s="3" t="str">
-        <f t="shared" ref="D238:D259" si="5">B238&amp;"_"&amp;C238</f>
+        <f t="shared" ref="D238:D262" si="5">B238&amp;"_"&amp;C238</f>
         <v>RXD_MACRO</v>
       </c>
       <c r="E238" s="3" t="s">
@@ -6756,6 +6846,552 @@
         <v>295</v>
       </c>
       <c r="F259" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A260" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B260" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D260" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>NSWNIMTOT_DEMOG</v>
+      </c>
+      <c r="E260" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F260" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D261" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>NSWNOMTOT_DEMOG</v>
+      </c>
+      <c r="E261" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F261" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B262" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D262" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>NSWNATTOT_DEMOG</v>
+      </c>
+      <c r="E262" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F262" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A263" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B263" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D263" s="2" t="str">
+        <f t="shared" ref="D263:D265" si="8">B263&amp;"_"&amp;C263</f>
+        <v>VICNIMTOT_DEMOG</v>
+      </c>
+      <c r="E263" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F263" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A264" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B264" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D264" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>VICNOMTOT_DEMOG</v>
+      </c>
+      <c r="E264" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F264" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A265" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B265" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D265" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>VICNATTOT_DEMOG</v>
+      </c>
+      <c r="E265" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F265" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B266" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D266" s="2" t="str">
+        <f t="shared" ref="D266:D271" si="9">B266&amp;"_"&amp;C266</f>
+        <v>QLDNIMTOT_DEMOG</v>
+      </c>
+      <c r="E266" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F266" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B267" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D267" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>QLDNOMTOT_DEMOG</v>
+      </c>
+      <c r="E267" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F267" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A268" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B268" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D268" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>QLDNATTOT_DEMOG</v>
+      </c>
+      <c r="E268" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F268" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A269" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B269" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D269" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>ACTNIMTOT_DEMOG</v>
+      </c>
+      <c r="E269" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F269" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A270" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B270" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D270" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>ACTNOMTOT_DEMOG</v>
+      </c>
+      <c r="E270" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F270" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A271" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B271" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D271" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>ACTNATTOT_DEMOG</v>
+      </c>
+      <c r="E271" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F271" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A272" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B272" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D272" s="2" t="str">
+        <f t="shared" ref="D272:D274" si="10">B272&amp;"_"&amp;C272</f>
+        <v>TASNIMTOT_DEMOG</v>
+      </c>
+      <c r="E272" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F272" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A273" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B273" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D273" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>TASNOMTOT_DEMOG</v>
+      </c>
+      <c r="E273" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F273" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A274" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B274" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D274" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>TASNATTOT_DEMOG</v>
+      </c>
+      <c r="E274" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F274" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A275" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B275" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D275" s="2" t="str">
+        <f t="shared" ref="D275:D277" si="11">B275&amp;"_"&amp;C275</f>
+        <v>SANIMTOT_DEMOG</v>
+      </c>
+      <c r="E275" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F275" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A276" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B276" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D276" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>SANOMTOT_DEMOG</v>
+      </c>
+      <c r="E276" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F276" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A277" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B277" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D277" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>SANATTOT_DEMOG</v>
+      </c>
+      <c r="E277" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F277" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A278" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B278" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D278" s="2" t="str">
+        <f t="shared" ref="D278:D280" si="12">B278&amp;"_"&amp;C278</f>
+        <v>NTNIMTOT_DEMOG</v>
+      </c>
+      <c r="E278" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F278" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A279" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B279" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D279" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>NTNOMTOT_DEMOG</v>
+      </c>
+      <c r="E279" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F279" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A280" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B280" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D280" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>NTNATTOT_DEMOG</v>
+      </c>
+      <c r="E280" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F280" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A281" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B281" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D281" s="2" t="str">
+        <f t="shared" ref="D281:D283" si="13">B281&amp;"_"&amp;C281</f>
+        <v>WANIMTOT_DEMOG</v>
+      </c>
+      <c r="E281" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F281" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A282" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B282" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D282" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>WANOMTOT_DEMOG</v>
+      </c>
+      <c r="E282" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F282" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A283" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B283" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D283" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>WANATTOT_DEMOG</v>
+      </c>
+      <c r="E283" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F283" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A284" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B284" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D284" s="2" t="str">
+        <f t="shared" ref="D284:D285" si="14">B284&amp;"_"&amp;C284</f>
+        <v>AUSNOMTOT_DEMOG</v>
+      </c>
+      <c r="E284" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F284" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A285" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B285" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D285" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>AUSNATTOT_DEMOG</v>
+      </c>
+      <c r="E285" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F285" s="2" t="s">
         <v>216</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding DEMOG to dashboard_data.rds
Adding NOM,NIM, NAT, POP INC data
</commit_message>
<xml_diff>
--- a/data processing/Input Files/List_of_Indicators.xlsx
+++ b/data processing/Input Files/List_of_Indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcrook\Documents\scenario_dashboard\data processing\Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC660A9C-CBFE-4B5B-985C-CC1F7F94C794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC6EBA5-108F-45C8-AAFF-4734F3C2CFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{794FE58A-84D8-4721-BA4E-C54580252300}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$259</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$285</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1394,10 +1394,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5594264D-85FA-45F5-B682-9D38B256CF42}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="F288" sqref="F288"/>
+    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6366,7 +6367,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="s">
         <v>209</v>
       </c>
@@ -6387,7 +6388,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="3" t="s">
         <v>209</v>
       </c>
@@ -6471,7 +6472,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>209</v>
       </c>
@@ -6492,7 +6493,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>209</v>
       </c>
@@ -6513,7 +6514,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>209</v>
       </c>
@@ -6534,7 +6535,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>209</v>
       </c>
@@ -6555,7 +6556,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>209</v>
       </c>
@@ -6576,7 +6577,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>209</v>
       </c>
@@ -6597,7 +6598,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>209</v>
       </c>
@@ -6618,7 +6619,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>209</v>
       </c>
@@ -6639,7 +6640,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>209</v>
       </c>
@@ -6660,7 +6661,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>209</v>
       </c>
@@ -6681,7 +6682,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>209</v>
       </c>
@@ -6702,7 +6703,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>209</v>
       </c>
@@ -6723,7 +6724,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>209</v>
       </c>
@@ -6744,7 +6745,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>209</v>
       </c>
@@ -6765,7 +6766,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>209</v>
       </c>
@@ -6786,7 +6787,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>209</v>
       </c>
@@ -6807,7 +6808,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>209</v>
       </c>
@@ -6828,7 +6829,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>209</v>
       </c>
@@ -7396,6 +7397,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F285" xr:uid="{5594264D-85FA-45F5-B682-9D38B256CF42}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="DEMOG"/>
+        <filter val="STATES"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding Demographics Breakdown Chart
</commit_message>
<xml_diff>
--- a/data processing/Input Files/List_of_Indicators.xlsx
+++ b/data processing/Input Files/List_of_Indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcrook\Documents\scenario_dashboard\data processing\Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC6EBA5-108F-45C8-AAFF-4734F3C2CFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69B0A30-28C8-4897-A672-7AEFAF4DB6EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{794FE58A-84D8-4721-BA4E-C54580252300}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="338">
   <si>
     <t>POPTOTTACT</t>
   </si>
@@ -1020,6 +1020,36 @@
   </si>
   <si>
     <t>AUSNATTOT</t>
+  </si>
+  <si>
+    <t>POPINC</t>
+  </si>
+  <si>
+    <t>AUSPOPINC</t>
+  </si>
+  <si>
+    <t>NSWPOPINC</t>
+  </si>
+  <si>
+    <t>VICPOPINC</t>
+  </si>
+  <si>
+    <t>QLDPOPINC</t>
+  </si>
+  <si>
+    <t>ACTPOPINC</t>
+  </si>
+  <si>
+    <t>TASPOPINC</t>
+  </si>
+  <si>
+    <t>SAPOPINC</t>
+  </si>
+  <si>
+    <t>NTPOPINC</t>
+  </si>
+  <si>
+    <t>WAPOPINC</t>
   </si>
 </sst>
 </file>
@@ -1395,10 +1425,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5594264D-85FA-45F5-B682-9D38B256CF42}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F285"/>
+  <dimension ref="A1:F294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A240" workbookViewId="0">
+      <selection activeCell="G286" sqref="G286:G294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7396,6 +7426,195 @@
         <v>216</v>
       </c>
     </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A286" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B286" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D286" s="2" t="str">
+        <f t="shared" ref="D286" si="15">B286&amp;"_"&amp;C286</f>
+        <v>AUSPOPINC_DEMOG</v>
+      </c>
+      <c r="E286" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="F286" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A287" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B287" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C287" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D287" s="2" t="str">
+        <f t="shared" ref="D287:D294" si="16">B287&amp;"_"&amp;C287</f>
+        <v>NSWPOPINC_DEMOG</v>
+      </c>
+      <c r="E287" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="F287" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A288" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B288" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C288" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D288" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>VICPOPINC_DEMOG</v>
+      </c>
+      <c r="E288" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="F288" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A289" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B289" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C289" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D289" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>QLDPOPINC_DEMOG</v>
+      </c>
+      <c r="E289" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="F289" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A290" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B290" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D290" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>ACTPOPINC_DEMOG</v>
+      </c>
+      <c r="E290" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="F290" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A291" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B291" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C291" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D291" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>TASPOPINC_DEMOG</v>
+      </c>
+      <c r="E291" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="F291" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A292" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B292" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D292" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>SAPOPINC_DEMOG</v>
+      </c>
+      <c r="E292" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="F292" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A293" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B293" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D293" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>NTPOPINC_DEMOG</v>
+      </c>
+      <c r="E293" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="F293" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A294" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B294" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D294" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>WAPOPINC_DEMOG</v>
+      </c>
+      <c r="E294" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="F294" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F285" xr:uid="{5594264D-85FA-45F5-B682-9D38B256CF42}">
     <filterColumn colId="2">

</xml_diff>

<commit_message>
updating to AEMO formatted bases
</commit_message>
<xml_diff>
--- a/data processing/Input Files/List_of_Indicators.xlsx
+++ b/data processing/Input Files/List_of_Indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcrook\Documents\scenario_dashboard\data processing\Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69B0A30-28C8-4897-A672-7AEFAF4DB6EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E33FAD7-1330-41AE-961C-2BB90B934FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{794FE58A-84D8-4721-BA4E-C54580252300}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$285</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$294</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="348">
   <si>
     <t>POPTOTTACT</t>
   </si>
@@ -1050,6 +1050,36 @@
   </si>
   <si>
     <t>WAPOPINC</t>
+  </si>
+  <si>
+    <t>GVAO_PLCCACT</t>
+  </si>
+  <si>
+    <t>GVAO_PLCCNSW</t>
+  </si>
+  <si>
+    <t>GVAO_PLCCQSL</t>
+  </si>
+  <si>
+    <t>GVAO_PLCCSAL</t>
+  </si>
+  <si>
+    <t>GVAO_PLCCTAS</t>
+  </si>
+  <si>
+    <t>GVAO_PLCCVIC</t>
+  </si>
+  <si>
+    <t>GVAO_PLCCNTY</t>
+  </si>
+  <si>
+    <t>GVAO_PLCCWAL</t>
+  </si>
+  <si>
+    <t>GVAO_PLCCAUS</t>
+  </si>
+  <si>
+    <t>GVAO_PLCC</t>
   </si>
 </sst>
 </file>
@@ -1425,10 +1455,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5594264D-85FA-45F5-B682-9D38B256CF42}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F294"/>
+  <dimension ref="A1:F303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A240" workbookViewId="0">
-      <selection activeCell="G286" sqref="G286:G294"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B235" sqref="B235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1462,7 +1492,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>209</v>
       </c>
@@ -1483,7 +1513,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>209</v>
       </c>
@@ -1504,7 +1534,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>209</v>
       </c>
@@ -1525,7 +1555,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>209</v>
       </c>
@@ -1546,7 +1576,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>209</v>
       </c>
@@ -1567,7 +1597,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>209</v>
       </c>
@@ -1588,7 +1618,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>209</v>
       </c>
@@ -1609,7 +1639,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>209</v>
       </c>
@@ -1630,7 +1660,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>209</v>
       </c>
@@ -1651,7 +1681,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>209</v>
       </c>
@@ -1672,7 +1702,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>209</v>
       </c>
@@ -1693,7 +1723,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>209</v>
       </c>
@@ -1714,7 +1744,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>209</v>
       </c>
@@ -1735,7 +1765,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>209</v>
       </c>
@@ -1756,7 +1786,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>209</v>
       </c>
@@ -1777,7 +1807,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>209</v>
       </c>
@@ -1798,7 +1828,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>209</v>
       </c>
@@ -1819,7 +1849,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>209</v>
       </c>
@@ -1840,7 +1870,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>209</v>
       </c>
@@ -1861,7 +1891,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>209</v>
       </c>
@@ -1882,7 +1912,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>209</v>
       </c>
@@ -1903,7 +1933,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>209</v>
       </c>
@@ -1924,7 +1954,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>209</v>
       </c>
@@ -1945,7 +1975,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>209</v>
       </c>
@@ -1966,7 +1996,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>209</v>
       </c>
@@ -2008,7 +2038,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>209</v>
       </c>
@@ -2029,7 +2059,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>209</v>
       </c>
@@ -2050,7 +2080,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>209</v>
       </c>
@@ -2071,7 +2101,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>209</v>
       </c>
@@ -2092,7 +2122,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>209</v>
       </c>
@@ -2113,7 +2143,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>209</v>
       </c>
@@ -2134,7 +2164,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>209</v>
       </c>
@@ -2155,7 +2185,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>209</v>
       </c>
@@ -2176,7 +2206,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>209</v>
       </c>
@@ -2197,7 +2227,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>209</v>
       </c>
@@ -2218,7 +2248,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>209</v>
       </c>
@@ -2239,7 +2269,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>209</v>
       </c>
@@ -2260,7 +2290,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>209</v>
       </c>
@@ -2281,7 +2311,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>209</v>
       </c>
@@ -2302,7 +2332,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>209</v>
       </c>
@@ -2323,7 +2353,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>209</v>
       </c>
@@ -2344,7 +2374,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>209</v>
       </c>
@@ -2365,7 +2395,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>209</v>
       </c>
@@ -2386,7 +2416,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>209</v>
       </c>
@@ -2407,7 +2437,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>209</v>
       </c>
@@ -2428,7 +2458,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>209</v>
       </c>
@@ -2449,7 +2479,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>209</v>
       </c>
@@ -2470,7 +2500,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>209</v>
       </c>
@@ -2491,7 +2521,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>209</v>
       </c>
@@ -2512,7 +2542,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>209</v>
       </c>
@@ -2554,7 +2584,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>209</v>
       </c>
@@ -2575,7 +2605,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>209</v>
       </c>
@@ -2596,7 +2626,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>209</v>
       </c>
@@ -2617,7 +2647,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>209</v>
       </c>
@@ -2638,7 +2668,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>209</v>
       </c>
@@ -2659,7 +2689,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>209</v>
       </c>
@@ -2680,7 +2710,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>209</v>
       </c>
@@ -2701,7 +2731,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>209</v>
       </c>
@@ -2722,7 +2752,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>209</v>
       </c>
@@ -2743,7 +2773,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>209</v>
       </c>
@@ -2764,7 +2794,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>209</v>
       </c>
@@ -2785,7 +2815,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>209</v>
       </c>
@@ -2806,7 +2836,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>209</v>
       </c>
@@ -2827,7 +2857,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>209</v>
       </c>
@@ -2848,7 +2878,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>209</v>
       </c>
@@ -2869,7 +2899,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>209</v>
       </c>
@@ -2890,7 +2920,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>209</v>
       </c>
@@ -2911,7 +2941,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>209</v>
       </c>
@@ -2932,7 +2962,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>209</v>
       </c>
@@ -2953,7 +2983,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>209</v>
       </c>
@@ -2974,7 +3004,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>209</v>
       </c>
@@ -2995,7 +3025,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>209</v>
       </c>
@@ -3016,7 +3046,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>209</v>
       </c>
@@ -3037,7 +3067,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>209</v>
       </c>
@@ -3058,7 +3088,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>209</v>
       </c>
@@ -3100,7 +3130,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>209</v>
       </c>
@@ -3121,7 +3151,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>209</v>
       </c>
@@ -3142,7 +3172,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>209</v>
       </c>
@@ -3163,7 +3193,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>209</v>
       </c>
@@ -3184,7 +3214,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>209</v>
       </c>
@@ -3205,7 +3235,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>209</v>
       </c>
@@ -3226,7 +3256,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>209</v>
       </c>
@@ -3247,7 +3277,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>209</v>
       </c>
@@ -3268,7 +3298,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>209</v>
       </c>
@@ -3289,7 +3319,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>209</v>
       </c>
@@ -3310,7 +3340,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>209</v>
       </c>
@@ -3331,7 +3361,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>209</v>
       </c>
@@ -3352,7 +3382,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>209</v>
       </c>
@@ -3373,7 +3403,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>209</v>
       </c>
@@ -3394,7 +3424,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>209</v>
       </c>
@@ -3415,7 +3445,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>209</v>
       </c>
@@ -3436,7 +3466,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>209</v>
       </c>
@@ -3457,7 +3487,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>209</v>
       </c>
@@ -3478,7 +3508,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>209</v>
       </c>
@@ -3499,7 +3529,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>209</v>
       </c>
@@ -3520,7 +3550,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>209</v>
       </c>
@@ -3541,7 +3571,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>209</v>
       </c>
@@ -3562,7 +3592,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>209</v>
       </c>
@@ -3583,7 +3613,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>209</v>
       </c>
@@ -3604,7 +3634,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>209</v>
       </c>
@@ -3646,7 +3676,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>209</v>
       </c>
@@ -3667,7 +3697,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>209</v>
       </c>
@@ -3688,7 +3718,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>209</v>
       </c>
@@ -3709,7 +3739,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>209</v>
       </c>
@@ -3730,7 +3760,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>209</v>
       </c>
@@ -3751,7 +3781,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>209</v>
       </c>
@@ -3772,7 +3802,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>209</v>
       </c>
@@ -3793,7 +3823,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>209</v>
       </c>
@@ -3814,7 +3844,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>209</v>
       </c>
@@ -3835,7 +3865,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>209</v>
       </c>
@@ -3856,7 +3886,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>209</v>
       </c>
@@ -3877,7 +3907,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>209</v>
       </c>
@@ -3898,7 +3928,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>209</v>
       </c>
@@ -3919,7 +3949,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>209</v>
       </c>
@@ -3940,7 +3970,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>209</v>
       </c>
@@ -3961,7 +3991,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>209</v>
       </c>
@@ -3982,7 +4012,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>209</v>
       </c>
@@ -4003,7 +4033,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>209</v>
       </c>
@@ -4024,7 +4054,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>209</v>
       </c>
@@ -4045,7 +4075,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>209</v>
       </c>
@@ -4066,7 +4096,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>209</v>
       </c>
@@ -4087,7 +4117,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>209</v>
       </c>
@@ -4108,7 +4138,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>209</v>
       </c>
@@ -4129,7 +4159,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>209</v>
       </c>
@@ -4150,7 +4180,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>209</v>
       </c>
@@ -4192,7 +4222,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>209</v>
       </c>
@@ -4213,7 +4243,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>209</v>
       </c>
@@ -4234,7 +4264,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>209</v>
       </c>
@@ -4255,7 +4285,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>209</v>
       </c>
@@ -4276,7 +4306,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>209</v>
       </c>
@@ -4297,7 +4327,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>209</v>
       </c>
@@ -4318,7 +4348,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>209</v>
       </c>
@@ -4339,7 +4369,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>209</v>
       </c>
@@ -4360,7 +4390,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>209</v>
       </c>
@@ -4381,7 +4411,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>209</v>
       </c>
@@ -4402,7 +4432,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>209</v>
       </c>
@@ -4423,7 +4453,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>209</v>
       </c>
@@ -4444,7 +4474,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>209</v>
       </c>
@@ -4465,7 +4495,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>209</v>
       </c>
@@ -4486,7 +4516,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>209</v>
       </c>
@@ -4507,7 +4537,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>209</v>
       </c>
@@ -4528,7 +4558,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>209</v>
       </c>
@@ -4549,7 +4579,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>209</v>
       </c>
@@ -4570,7 +4600,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>209</v>
       </c>
@@ -4591,7 +4621,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>209</v>
       </c>
@@ -4612,7 +4642,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>209</v>
       </c>
@@ -4633,7 +4663,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>209</v>
       </c>
@@ -4654,7 +4684,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>209</v>
       </c>
@@ -4675,7 +4705,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>209</v>
       </c>
@@ -4696,7 +4726,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>209</v>
       </c>
@@ -4738,7 +4768,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>209</v>
       </c>
@@ -4759,7 +4789,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>209</v>
       </c>
@@ -4780,7 +4810,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>209</v>
       </c>
@@ -4801,7 +4831,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>209</v>
       </c>
@@ -4822,7 +4852,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>209</v>
       </c>
@@ -4843,7 +4873,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>209</v>
       </c>
@@ -4864,7 +4894,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>209</v>
       </c>
@@ -4885,7 +4915,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>209</v>
       </c>
@@ -4906,7 +4936,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>209</v>
       </c>
@@ -4927,7 +4957,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>209</v>
       </c>
@@ -4948,7 +4978,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>209</v>
       </c>
@@ -4969,7 +4999,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>209</v>
       </c>
@@ -4990,7 +5020,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>209</v>
       </c>
@@ -5011,7 +5041,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>209</v>
       </c>
@@ -5032,7 +5062,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>209</v>
       </c>
@@ -5053,7 +5083,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>209</v>
       </c>
@@ -5074,7 +5104,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>209</v>
       </c>
@@ -5095,7 +5125,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>209</v>
       </c>
@@ -5116,7 +5146,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>209</v>
       </c>
@@ -5137,7 +5167,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>209</v>
       </c>
@@ -5158,7 +5188,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>209</v>
       </c>
@@ -5179,7 +5209,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>209</v>
       </c>
@@ -5200,7 +5230,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>209</v>
       </c>
@@ -5221,7 +5251,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>209</v>
       </c>
@@ -5242,7 +5272,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>209</v>
       </c>
@@ -5284,7 +5314,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>209</v>
       </c>
@@ -5305,7 +5335,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>209</v>
       </c>
@@ -5326,7 +5356,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>209</v>
       </c>
@@ -5347,7 +5377,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>209</v>
       </c>
@@ -5368,7 +5398,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>209</v>
       </c>
@@ -5389,7 +5419,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>209</v>
       </c>
@@ -5410,7 +5440,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>209</v>
       </c>
@@ -5431,7 +5461,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>209</v>
       </c>
@@ -5452,7 +5482,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>209</v>
       </c>
@@ -5473,7 +5503,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>209</v>
       </c>
@@ -5494,7 +5524,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>209</v>
       </c>
@@ -5515,7 +5545,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>209</v>
       </c>
@@ -5536,7 +5566,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>209</v>
       </c>
@@ -5557,7 +5587,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>209</v>
       </c>
@@ -5578,7 +5608,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>209</v>
       </c>
@@ -5599,7 +5629,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>209</v>
       </c>
@@ -5620,7 +5650,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>209</v>
       </c>
@@ -5641,7 +5671,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>209</v>
       </c>
@@ -5662,7 +5692,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>209</v>
       </c>
@@ -5683,7 +5713,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>209</v>
       </c>
@@ -5704,7 +5734,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>209</v>
       </c>
@@ -5725,7 +5755,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>209</v>
       </c>
@@ -5746,7 +5776,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>209</v>
       </c>
@@ -5767,7 +5797,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>209</v>
       </c>
@@ -5788,7 +5818,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>209</v>
       </c>
@@ -5830,7 +5860,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>209</v>
       </c>
@@ -5851,7 +5881,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>209</v>
       </c>
@@ -5872,7 +5902,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>209</v>
       </c>
@@ -5893,7 +5923,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>209</v>
       </c>
@@ -5914,7 +5944,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>209</v>
       </c>
@@ -5935,7 +5965,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>209</v>
       </c>
@@ -5956,7 +5986,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>209</v>
       </c>
@@ -5977,7 +6007,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>209</v>
       </c>
@@ -5998,7 +6028,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>209</v>
       </c>
@@ -6019,7 +6049,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>209</v>
       </c>
@@ -6040,7 +6070,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>209</v>
       </c>
@@ -6061,7 +6091,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>209</v>
       </c>
@@ -6082,7 +6112,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>209</v>
       </c>
@@ -6103,7 +6133,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>209</v>
       </c>
@@ -6124,7 +6154,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>209</v>
       </c>
@@ -6145,7 +6175,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>209</v>
       </c>
@@ -6166,7 +6196,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>209</v>
       </c>
@@ -6187,7 +6217,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>209</v>
       </c>
@@ -6208,7 +6238,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>209</v>
       </c>
@@ -6229,7 +6259,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>209</v>
       </c>
@@ -6250,7 +6280,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>209</v>
       </c>
@@ -6271,7 +6301,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>209</v>
       </c>
@@ -6292,7 +6322,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>209</v>
       </c>
@@ -6313,7 +6343,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>209</v>
       </c>
@@ -6334,7 +6364,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>209</v>
       </c>
@@ -6376,7 +6406,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>209</v>
       </c>
@@ -6439,7 +6469,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>209</v>
       </c>
@@ -6460,7 +6490,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>209</v>
       </c>
@@ -6481,7 +6511,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>209</v>
       </c>
@@ -6880,7 +6910,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>209</v>
       </c>
@@ -6901,7 +6931,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>209</v>
       </c>
@@ -6922,7 +6952,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>209</v>
       </c>
@@ -6943,7 +6973,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>209</v>
       </c>
@@ -6964,7 +6994,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>209</v>
       </c>
@@ -6985,7 +7015,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>209</v>
       </c>
@@ -7006,7 +7036,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>209</v>
       </c>
@@ -7027,7 +7057,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>209</v>
       </c>
@@ -7048,7 +7078,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>209</v>
       </c>
@@ -7069,7 +7099,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>209</v>
       </c>
@@ -7090,7 +7120,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>209</v>
       </c>
@@ -7111,7 +7141,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>209</v>
       </c>
@@ -7132,7 +7162,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>209</v>
       </c>
@@ -7153,7 +7183,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>209</v>
       </c>
@@ -7174,7 +7204,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>209</v>
       </c>
@@ -7195,7 +7225,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>209</v>
       </c>
@@ -7216,7 +7246,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>209</v>
       </c>
@@ -7237,7 +7267,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>209</v>
       </c>
@@ -7258,7 +7288,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>209</v>
       </c>
@@ -7279,7 +7309,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>209</v>
       </c>
@@ -7300,7 +7330,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
         <v>209</v>
       </c>
@@ -7321,7 +7351,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>209</v>
       </c>
@@ -7342,7 +7372,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>209</v>
       </c>
@@ -7363,7 +7393,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>209</v>
       </c>
@@ -7384,7 +7414,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>209</v>
       </c>
@@ -7405,7 +7435,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>209</v>
       </c>
@@ -7426,7 +7456,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>209</v>
       </c>
@@ -7447,7 +7477,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
         <v>209</v>
       </c>
@@ -7458,7 +7488,7 @@
         <v>298</v>
       </c>
       <c r="D287" s="2" t="str">
-        <f t="shared" ref="D287:D294" si="16">B287&amp;"_"&amp;C287</f>
+        <f t="shared" ref="D287:D303" si="16">B287&amp;"_"&amp;C287</f>
         <v>NSWPOPINC_DEMOG</v>
       </c>
       <c r="E287" s="2" t="s">
@@ -7468,7 +7498,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>209</v>
       </c>
@@ -7489,7 +7519,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>209</v>
       </c>
@@ -7510,7 +7540,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
         <v>209</v>
       </c>
@@ -7531,7 +7561,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
         <v>209</v>
       </c>
@@ -7552,7 +7582,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
         <v>209</v>
       </c>
@@ -7573,7 +7603,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
         <v>209</v>
       </c>
@@ -7594,7 +7624,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
         <v>209</v>
       </c>
@@ -7615,11 +7645,212 @@
         <v>216</v>
       </c>
     </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A295" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B295" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C295" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D295" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>GVAO_PLCCACT_STATES</v>
+      </c>
+      <c r="E295" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F295" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A296" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B296" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C296" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D296" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>GVAO_PLCCNSW_STATES</v>
+      </c>
+      <c r="E296" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F296" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A297" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B297" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D297" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>GVAO_PLCCQSL_STATES</v>
+      </c>
+      <c r="E297" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F297" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A298" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B298" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D298" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>GVAO_PLCCSAL_STATES</v>
+      </c>
+      <c r="E298" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F298" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A299" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B299" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C299" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D299" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>GVAO_PLCCTAS_STATES</v>
+      </c>
+      <c r="E299" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F299" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A300" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B300" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C300" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D300" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>GVAO_PLCCVIC_STATES</v>
+      </c>
+      <c r="E300" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F300" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A301" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B301" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D301" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>GVAO_PLCCNTY_STATES</v>
+      </c>
+      <c r="E301" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F301" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A302" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B302" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="C302" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D302" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>GVAO_PLCCWAL_STATES</v>
+      </c>
+      <c r="E302" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F302" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A303" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B303" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C303" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D303" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>GVAO_PLCCAUS_STATES</v>
+      </c>
+      <c r="E303" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F303" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F285" xr:uid="{5594264D-85FA-45F5-B682-9D38B256CF42}">
+  <autoFilter ref="A1:F294" xr:uid="{5594264D-85FA-45F5-B682-9D38B256CF42}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="GVAOLCCACT"/>
+        <filter val="GVAOLCCAUS"/>
+        <filter val="GVAOLCCNSW"/>
+        <filter val="GVAOLCCNTY"/>
+        <filter val="GVAOLCCQSL"/>
+        <filter val="GVAOLCCSAL"/>
+        <filter val="GVAOLCCTAS"/>
+        <filter val="GVAOLCCVIC"/>
+        <filter val="GVAOLCCWAL"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="2">
       <filters>
-        <filter val="DEMOG"/>
         <filter val="STATES"/>
       </filters>
     </filterColumn>

</xml_diff>